<commit_message>
yo digo que ya esta esa mierda, hay unos bugs :v
</commit_message>
<xml_diff>
--- a/WineCompany2.xlsx
+++ b/WineCompany2.xlsx
@@ -1,9 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldair Estrada\Documents\2S 2020\Modelacion y Simulacion 1\Clase Laboratorio\Proyecto\PModela\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA5ACC2-9AAB-45A6-AD64-02B1AB366017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elaboracion_Vino" sheetId="1" r:id="rId1"/>
@@ -15,33 +22,34 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
           <t>Tipo de uva:</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>_x000A_1 -&gt; Palomino_x000A_2 -&gt; Cariñena_x000A_3 -&gt; Tinta Barroca</t>
+          <t xml:space="preserve">
+1 -&gt; Palomino
+2 -&gt; Cariñena
+3 -&gt; Tinta Barroca</t>
         </r>
       </text>
     </comment>
@@ -50,97 +58,106 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
           <t>Tipo de orden:</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>_x000A_0 -&gt; Cliente_x000A_1 -&gt; Tienda 1_x000A_2 -&gt; Tienda 2_x000A_3 -&gt; Tienda 3_x000A_4 -&gt; Tienda 4_x000A_5 -&gt; Tienda 5</t>
+          <t xml:space="preserve">
+0 -&gt; Cliente
+1 -&gt; Tienda 1
+2 -&gt; Tienda 2
+3 -&gt; Tienda 3
+4 -&gt; Tienda 4
+5 -&gt; Tienda 5</t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
           <t>Tipo de vino:</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>_x000A_1 -&gt; Vino Blanco_x000A_2 -&gt; Vino Tinto_x000A_3 -&gt; Vino Oporto_x000A_4 -&gt; Vino Jerez_x000A_5 -&gt; Vino Rosado</t>
+          <t xml:space="preserve">
+1 -&gt; Vino Blanco
+2 -&gt; Vino Tinto
+3 -&gt; Vino Oporto
+4 -&gt; Vino Jerez
+5 -&gt; Vino Rosado</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
           <t>Tipo de botella:</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>_x000A_1 -&gt; Estándar_x000A_2 -&gt; Magnum_x000A_3 -&gt; Doble Magnum_x000A_4 -&gt; Imperial</t>
+          <t xml:space="preserve">
+1 -&gt; Estándar
+2 -&gt; Magnum
+3 -&gt; Doble Magnum
+4 -&gt; Imperial</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>La cantidad de botellas siempre es un múltiplo de la capacidade de las cajas_x000A_</t>
+          <t xml:space="preserve">La cantidad de botellas siempre es un múltiplo de la capacidade de las cajas
+</t>
         </r>
       </text>
     </comment>
@@ -149,48 +166,55 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Usuario de Windows</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>Tipo de vino:_x000A_1 -&gt; Vino Blanco_x000A_2 -&gt; Vino Tinto_x000A_3 -&gt; Vino Oporto_x000A_4 -&gt; Vino Jerez_x000A_5 -&gt; Vino Rosado</t>
+          <t>Tipo de vino:
+1 -&gt; Vino Blanco
+2 -&gt; Vino Tinto
+3 -&gt; Vino Oporto
+4 -&gt; Vino Jerez
+5 -&gt; Vino Rosado</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <b val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>Tipo de botella:_x000A_1 -&gt; Estándar_x000A_2 -&gt; Magnum_x000A_3 -&gt; Doble Magnum_x000A_4 -&gt; Imperial</t>
+          <t>Tipo de botella:
+1 -&gt; Estándar
+2 -&gt; Magnum
+3 -&gt; Doble Magnum
+4 -&gt; Imperial</t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <charset val="1"/>
-            <color indexed="81"/>
-            <sz val="9"/>
-            <scheme val="none"/>
           </rPr>
-          <t>_x000A_</t>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -199,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Tipo de Uva</t>
   </si>
@@ -228,8 +252,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,6 +268,19 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -254,7 +291,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -269,6 +312,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -277,10 +328,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -526,23 +577,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42188" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.71094" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -558,7 +612,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -566,7 +620,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -575,28 +629,30 @@
       </c>
     </row>
   </sheetData>
-  <pageSetup r:id="rId1" paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.14063" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -613,12 +669,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -630,12 +686,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -647,12 +703,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -664,12 +720,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -681,12 +737,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -698,12 +754,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -715,12 +771,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -732,12 +788,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -749,12 +805,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -766,12 +822,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -783,12 +839,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -800,12 +856,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -817,12 +873,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -834,7 +890,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -851,7 +907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -868,7 +924,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -885,7 +941,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -902,7 +958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -919,7 +975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -936,7 +992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -953,7 +1009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -970,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -987,7 +1043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1004,7 +1060,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1021,7 +1077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1038,7 +1094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1055,7 +1111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1072,7 +1128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1089,7 +1145,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1106,7 +1162,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1123,7 +1179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1140,7 +1196,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>7</v>
       </c>
@@ -1157,7 +1213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7</v>
       </c>
@@ -1174,7 +1230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7</v>
       </c>
@@ -1191,7 +1247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -1208,7 +1264,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7</v>
       </c>
@@ -1226,25 +1282,27 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.14063" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1255,7 +1313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1266,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1277,7 +1335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1288,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1299,7 +1357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1310,7 +1368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1321,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1332,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1343,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1354,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1366,7 +1424,8 @@
       </c>
     </row>
   </sheetData>
-  <pageSetup r:id="rId1" paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>